<commit_message>
Deploying to gh-pages from @ wanghuaijin/wanghuaijin.github.io@e9d88e4066e6fe346187d58847cac2829b8f234f 🚀
</commit_message>
<xml_diff>
--- a/assets/numDEs/status/evaluation.xlsx
+++ b/assets/numDEs/status/evaluation.xlsx
@@ -654,7 +654,7 @@
     <t>73%</t>
   </si>
   <si>
-    <t>91%</t>
+    <t>96%</t>
   </si>
   <si>
     <t>58%</t>
@@ -672,7 +672,7 @@
     <t>89%</t>
   </si>
   <si>
-    <t>64%</t>
+    <t>69%</t>
   </si>
   <si>
     <t>93%</t>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ wanghuaijin/wanghuaijin.github.io@347194349fe4088fcb4c9509c31bd151932327a5 🚀
</commit_message>
<xml_diff>
--- a/assets/numDEs/status/evaluation.xlsx
+++ b/assets/numDEs/status/evaluation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="11380"/>
+    <workbookView windowWidth="28000" windowHeight="12860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="212">
   <si>
     <t>序号</t>
   </si>
@@ -206,7 +206,7 @@
     <t>刘清华</t>
   </si>
   <si>
-    <t>51%</t>
+    <t>69%</t>
   </si>
   <si>
     <t>65%</t>
@@ -336,9 +336,6 @@
   </si>
   <si>
     <t>85%</t>
-  </si>
-  <si>
-    <t>69%</t>
   </si>
   <si>
     <t>20420202201837</t>
@@ -1821,19 +1818,20 @@
   <sheetPr/>
   <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="7.9296875" customWidth="1"/>
-    <col min="4" max="4" width="14.96875" customWidth="1"/>
-    <col min="5" max="5" width="17.9609375" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="8" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.4453125" customWidth="1"/>
+    <col min="4" max="4" width="18.875" customWidth="1"/>
+    <col min="5" max="5" width="21.4765625" customWidth="1"/>
+    <col min="6" max="6" width="13.9296875" customWidth="1"/>
+    <col min="7" max="7" width="14.8359375" customWidth="1"/>
+    <col min="8" max="8" width="17.3125" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2559,7 +2557,7 @@
         <v>102</v>
       </c>
       <c r="I25" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2567,19 +2565,19 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" t="s">
         <v>104</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
         <v>105</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>106</v>
       </c>
       <c r="G26" t="s">
         <v>32</v>
@@ -2588,7 +2586,7 @@
         <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2596,10 +2594,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" t="s">
         <v>108</v>
-      </c>
-      <c r="C27" t="s">
-        <v>109</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -2625,19 +2623,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" t="s">
         <v>110</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
         <v>111</v>
-      </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
-        <v>112</v>
       </c>
       <c r="G28" t="s">
         <v>73</v>
@@ -2654,16 +2652,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C29" t="s">
         <v>113</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
         <v>114</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" t="s">
-        <v>115</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
@@ -2683,10 +2681,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>115</v>
+      </c>
+      <c r="C30" t="s">
         <v>116</v>
-      </c>
-      <c r="C30" t="s">
-        <v>117</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -2712,10 +2710,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" t="s">
         <v>118</v>
-      </c>
-      <c r="C31" t="s">
-        <v>119</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2741,19 +2739,19 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>119</v>
+      </c>
+      <c r="C32" t="s">
         <v>120</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
         <v>121</v>
-      </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" t="s">
-        <v>122</v>
       </c>
       <c r="G32" t="s">
         <v>60</v>
@@ -2770,10 +2768,10 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
         <v>123</v>
-      </c>
-      <c r="C33" t="s">
-        <v>124</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -2799,10 +2797,10 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>124</v>
+      </c>
+      <c r="C34" t="s">
         <v>125</v>
-      </c>
-      <c r="C34" t="s">
-        <v>126</v>
       </c>
       <c r="D34" t="s">
         <v>11</v>
@@ -2828,19 +2826,19 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" t="s">
         <v>127</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
         <v>128</v>
-      </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" t="s">
-        <v>129</v>
       </c>
       <c r="G35" t="s">
         <v>24</v>
@@ -2857,19 +2855,19 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" t="s">
         <v>130</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" t="s">
         <v>131</v>
-      </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" t="s">
-        <v>132</v>
       </c>
       <c r="G36" t="s">
         <v>68</v>
@@ -2886,10 +2884,10 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" t="s">
         <v>133</v>
-      </c>
-      <c r="C37" t="s">
-        <v>134</v>
       </c>
       <c r="D37" t="s">
         <v>11</v>
@@ -2915,19 +2913,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" t="s">
         <v>135</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
         <v>136</v>
-      </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" t="s">
-        <v>137</v>
       </c>
       <c r="G38" t="s">
         <v>19</v>
@@ -2944,10 +2942,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" t="s">
         <v>138</v>
-      </c>
-      <c r="C39" t="s">
-        <v>139</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -2965,7 +2963,7 @@
         <v>24</v>
       </c>
       <c r="I39" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2973,10 +2971,10 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>140</v>
+      </c>
+      <c r="C40" t="s">
         <v>141</v>
-      </c>
-      <c r="C40" t="s">
-        <v>142</v>
       </c>
       <c r="D40" t="s">
         <v>11</v>
@@ -3002,10 +3000,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" t="s">
         <v>143</v>
-      </c>
-      <c r="C41" t="s">
-        <v>144</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -3031,10 +3029,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" t="s">
         <v>145</v>
-      </c>
-      <c r="C42" t="s">
-        <v>146</v>
       </c>
       <c r="D42" t="s">
         <v>11</v>
@@ -3060,19 +3058,19 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>146</v>
+      </c>
+      <c r="C43" t="s">
         <v>147</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" t="s">
         <v>148</v>
-      </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" t="s">
-        <v>149</v>
       </c>
       <c r="G43" t="s">
         <v>73</v>
@@ -3089,11 +3087,11 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>149</v>
+      </c>
+      <c r="C44" t="s">
         <v>150</v>
       </c>
-      <c r="C44" t="s">
-        <v>151</v>
-      </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
@@ -3101,7 +3099,7 @@
         <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G44" t="s">
         <v>18</v>
@@ -3118,10 +3116,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" t="s">
         <v>152</v>
-      </c>
-      <c r="C45" t="s">
-        <v>153</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -3147,11 +3145,11 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>153</v>
+      </c>
+      <c r="C46" t="s">
         <v>154</v>
       </c>
-      <c r="C46" t="s">
-        <v>155</v>
-      </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
@@ -3159,7 +3157,7 @@
         <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G46" t="s">
         <v>19</v>
@@ -3176,10 +3174,10 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" t="s">
         <v>156</v>
-      </c>
-      <c r="C47" t="s">
-        <v>157</v>
       </c>
       <c r="D47" t="s">
         <v>11</v>
@@ -3205,19 +3203,19 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" t="s">
         <v>158</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" t="s">
         <v>159</v>
-      </c>
-      <c r="D48" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" t="s">
-        <v>160</v>
       </c>
       <c r="G48" t="s">
         <v>32</v>
@@ -3234,19 +3232,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>160</v>
+      </c>
+      <c r="C49" t="s">
         <v>161</v>
       </c>
-      <c r="C49" t="s">
-        <v>162</v>
-      </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F49" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G49" t="s">
         <v>37</v>
@@ -3263,19 +3261,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>162</v>
+      </c>
+      <c r="C50" t="s">
         <v>163</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
         <v>164</v>
-      </c>
-      <c r="D50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" t="s">
-        <v>165</v>
       </c>
       <c r="G50" t="s">
         <v>19</v>
@@ -3292,19 +3290,19 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>165</v>
+      </c>
+      <c r="C51" t="s">
         <v>166</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
         <v>167</v>
-      </c>
-      <c r="D51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" t="s">
-        <v>168</v>
       </c>
       <c r="G51" t="s">
         <v>60</v>
@@ -3321,10 +3319,10 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>168</v>
+      </c>
+      <c r="C52" t="s">
         <v>169</v>
-      </c>
-      <c r="C52" t="s">
-        <v>170</v>
       </c>
       <c r="D52" t="s">
         <v>11</v>
@@ -3350,10 +3348,10 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>170</v>
+      </c>
+      <c r="C53" t="s">
         <v>171</v>
-      </c>
-      <c r="C53" t="s">
-        <v>172</v>
       </c>
       <c r="D53" t="s">
         <v>11</v>
@@ -3379,16 +3377,16 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>172</v>
+      </c>
+      <c r="C54" t="s">
         <v>173</v>
       </c>
-      <c r="C54" t="s">
-        <v>174</v>
-      </c>
       <c r="D54" t="s">
         <v>11</v>
       </c>
       <c r="E54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F54" t="s">
         <v>98</v>
@@ -3408,10 +3406,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>174</v>
+      </c>
+      <c r="C55" t="s">
         <v>175</v>
-      </c>
-      <c r="C55" t="s">
-        <v>176</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -3437,19 +3435,19 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" t="s">
         <v>177</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" t="s">
         <v>178</v>
-      </c>
-      <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
-        <v>12</v>
-      </c>
-      <c r="F56" t="s">
-        <v>179</v>
       </c>
       <c r="G56" t="s">
         <v>102</v>
@@ -3458,7 +3456,7 @@
         <v>24</v>
       </c>
       <c r="I56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -3466,19 +3464,19 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>179</v>
+      </c>
+      <c r="C57" t="s">
         <v>180</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
         <v>181</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" t="s">
-        <v>182</v>
       </c>
       <c r="G57" t="s">
         <v>18</v>
@@ -3495,11 +3493,11 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>182</v>
+      </c>
+      <c r="C58" t="s">
         <v>183</v>
       </c>
-      <c r="C58" t="s">
-        <v>184</v>
-      </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
@@ -3507,7 +3505,7 @@
         <v>12</v>
       </c>
       <c r="F58" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G58" t="s">
         <v>32</v>
@@ -3524,11 +3522,11 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>184</v>
+      </c>
+      <c r="C59" t="s">
         <v>185</v>
       </c>
-      <c r="C59" t="s">
-        <v>186</v>
-      </c>
       <c r="D59" t="s">
         <v>11</v>
       </c>
@@ -3536,7 +3534,7 @@
         <v>12</v>
       </c>
       <c r="F59" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G59" t="s">
         <v>24</v>
@@ -3553,10 +3551,10 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>186</v>
+      </c>
+      <c r="C60" t="s">
         <v>187</v>
-      </c>
-      <c r="C60" t="s">
-        <v>188</v>
       </c>
       <c r="D60" t="s">
         <v>11</v>
@@ -3582,19 +3580,19 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>188</v>
+      </c>
+      <c r="C61" t="s">
         <v>189</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" t="s">
         <v>190</v>
-      </c>
-      <c r="D61" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61" t="s">
-        <v>191</v>
       </c>
       <c r="G61" t="s">
         <v>60</v>
@@ -3611,10 +3609,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>191</v>
+      </c>
+      <c r="C62" t="s">
         <v>192</v>
-      </c>
-      <c r="C62" t="s">
-        <v>193</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -3640,11 +3638,11 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>193</v>
+      </c>
+      <c r="C63" t="s">
         <v>194</v>
       </c>
-      <c r="C63" t="s">
-        <v>195</v>
-      </c>
       <c r="D63" t="s">
         <v>11</v>
       </c>
@@ -3652,7 +3650,7 @@
         <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>103</v>
+        <v>59</v>
       </c>
       <c r="G63" t="s">
         <v>32</v>
@@ -3661,7 +3659,7 @@
         <v>73</v>
       </c>
       <c r="I63" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3669,11 +3667,11 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>195</v>
+      </c>
+      <c r="C64" t="s">
         <v>196</v>
       </c>
-      <c r="C64" t="s">
-        <v>197</v>
-      </c>
       <c r="D64" t="s">
         <v>11</v>
       </c>
@@ -3681,7 +3679,7 @@
         <v>12</v>
       </c>
       <c r="F64" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G64" t="s">
         <v>60</v>
@@ -3698,19 +3696,19 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>197</v>
+      </c>
+      <c r="C65" t="s">
         <v>198</v>
       </c>
-      <c r="C65" t="s">
-        <v>199</v>
-      </c>
       <c r="D65" t="s">
         <v>11</v>
       </c>
       <c r="E65" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G65" t="s">
         <v>77</v>
@@ -3727,10 +3725,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>199</v>
+      </c>
+      <c r="C66" t="s">
         <v>200</v>
-      </c>
-      <c r="C66" t="s">
-        <v>201</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
@@ -3756,11 +3754,11 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>201</v>
+      </c>
+      <c r="C67" t="s">
         <v>202</v>
       </c>
-      <c r="C67" t="s">
-        <v>203</v>
-      </c>
       <c r="D67" t="s">
         <v>11</v>
       </c>
@@ -3768,7 +3766,7 @@
         <v>12</v>
       </c>
       <c r="F67" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G67" t="s">
         <v>42</v>
@@ -3785,10 +3783,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>203</v>
+      </c>
+      <c r="C68" t="s">
         <v>204</v>
-      </c>
-      <c r="C68" t="s">
-        <v>205</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
@@ -3814,10 +3812,10 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>205</v>
+      </c>
+      <c r="C69" t="s">
         <v>206</v>
-      </c>
-      <c r="C69" t="s">
-        <v>207</v>
       </c>
       <c r="D69" t="s">
         <v>11</v>
@@ -3843,10 +3841,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>207</v>
+      </c>
+      <c r="C70" t="s">
         <v>208</v>
-      </c>
-      <c r="C70" t="s">
-        <v>209</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
@@ -3872,10 +3870,10 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>209</v>
+      </c>
+      <c r="C71" t="s">
         <v>210</v>
-      </c>
-      <c r="C71" t="s">
-        <v>211</v>
       </c>
       <c r="D71" t="s">
         <v>11</v>
@@ -3898,7 +3896,7 @@
     </row>
     <row r="73" spans="2:2">
       <c r="B73" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ wanghuaijin/wanghuaijin.github.io@3d02a26b4d89cce864ba476cab89cc3ef4c45612 🚀
</commit_message>
<xml_diff>
--- a/assets/numDEs/status/evaluation.xlsx
+++ b/assets/numDEs/status/evaluation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="211">
   <si>
     <t>序号</t>
   </si>
@@ -195,9 +195,6 @@
   </si>
   <si>
     <t>蒋志轩</t>
-  </si>
-  <si>
-    <t>37%</t>
   </si>
   <si>
     <t>19020212203453</t>
@@ -1819,19 +1816,18 @@
   <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A40" sqref="$A40:$XFD40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.4453125" customWidth="1"/>
-    <col min="4" max="4" width="18.875" customWidth="1"/>
-    <col min="5" max="5" width="21.4765625" customWidth="1"/>
-    <col min="6" max="6" width="13.9296875" customWidth="1"/>
-    <col min="7" max="7" width="14.8359375" customWidth="1"/>
-    <col min="8" max="8" width="17.3125" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" customWidth="1"/>
+    <col min="4" max="4" width="18.359375" customWidth="1"/>
+    <col min="5" max="5" width="14.8359375" customWidth="1"/>
+    <col min="6" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="8" width="6.7109375" customWidth="1"/>
     <col min="9" max="9" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2171,7 +2167,7 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s">
         <v>37</v>
@@ -2188,28 +2184,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
         <v>57</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
         <v>58</v>
       </c>
-      <c r="D13" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>59</v>
-      </c>
-      <c r="G13" t="s">
-        <v>60</v>
       </c>
       <c r="H13" t="s">
         <v>18</v>
       </c>
       <c r="I13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -2217,19 +2213,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" t="s">
         <v>62</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
         <v>63</v>
-      </c>
-      <c r="D14" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>64</v>
       </c>
       <c r="G14" t="s">
         <v>37</v>
@@ -2238,7 +2234,7 @@
         <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -2246,10 +2242,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" t="s">
         <v>66</v>
-      </c>
-      <c r="C15" t="s">
-        <v>67</v>
       </c>
       <c r="D15" t="s">
         <v>11</v>
@@ -2261,13 +2257,13 @@
         <v>23</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H15" t="s">
         <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -2275,19 +2271,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" t="s">
         <v>70</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
         <v>71</v>
-      </c>
-      <c r="D16" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>72</v>
       </c>
       <c r="G16" t="s">
         <v>32</v>
@@ -2296,7 +2292,7 @@
         <v>18</v>
       </c>
       <c r="I16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:9">
@@ -2304,25 +2300,25 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" t="s">
         <v>74</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
         <v>75</v>
-      </c>
-      <c r="D17" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>76</v>
       </c>
       <c r="G17" t="s">
         <v>19</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I17" t="s">
         <v>43</v>
@@ -2333,10 +2329,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s">
         <v>78</v>
-      </c>
-      <c r="C18" t="s">
-        <v>79</v>
       </c>
       <c r="D18" t="s">
         <v>11</v>
@@ -2362,28 +2358,28 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
         <v>81</v>
-      </c>
-      <c r="D19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" t="s">
-        <v>82</v>
       </c>
       <c r="G19" t="s">
         <v>19</v>
       </c>
       <c r="H19" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" t="s">
         <v>82</v>
-      </c>
-      <c r="I19" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -2391,19 +2387,19 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
         <v>84</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
         <v>85</v>
-      </c>
-      <c r="D20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>86</v>
       </c>
       <c r="G20" t="s">
         <v>32</v>
@@ -2420,19 +2416,19 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" t="s">
         <v>87</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
         <v>88</v>
-      </c>
-      <c r="D21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" t="s">
-        <v>89</v>
       </c>
       <c r="G21" t="s">
         <v>32</v>
@@ -2441,7 +2437,7 @@
         <v>32</v>
       </c>
       <c r="I21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -2449,10 +2445,10 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
         <v>90</v>
-      </c>
-      <c r="C22" t="s">
-        <v>91</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -2470,7 +2466,7 @@
         <v>32</v>
       </c>
       <c r="I22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:9">
@@ -2478,19 +2474,19 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" t="s">
         <v>93</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
         <v>94</v>
-      </c>
-      <c r="D23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" t="s">
-        <v>95</v>
       </c>
       <c r="G23" t="s">
         <v>24</v>
@@ -2499,7 +2495,7 @@
         <v>42</v>
       </c>
       <c r="I23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="24" spans="1:9">
@@ -2507,19 +2503,19 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C24" t="s">
         <v>96</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
         <v>97</v>
-      </c>
-      <c r="D24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" t="s">
-        <v>98</v>
       </c>
       <c r="G24" t="s">
         <v>19</v>
@@ -2528,7 +2524,7 @@
         <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:9">
@@ -2536,28 +2532,28 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
         <v>99</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
         <v>100</v>
-      </c>
-      <c r="D25" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" t="s">
-        <v>101</v>
       </c>
       <c r="G25" t="s">
         <v>50</v>
       </c>
       <c r="H25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="26" spans="1:9">
@@ -2565,28 +2561,28 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C26" t="s">
         <v>103</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
         <v>104</v>
-      </c>
-      <c r="D26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>105</v>
       </c>
       <c r="G26" t="s">
         <v>32</v>
       </c>
       <c r="H26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I26" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -2594,10 +2590,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
         <v>107</v>
-      </c>
-      <c r="C27" t="s">
-        <v>108</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -2609,13 +2605,13 @@
         <v>20</v>
       </c>
       <c r="G27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:9">
@@ -2623,28 +2619,28 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" t="s">
         <v>109</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
         <v>110</v>
       </c>
-      <c r="D28" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
-        <v>111</v>
-      </c>
       <c r="G28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:9">
@@ -2652,16 +2648,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" t="s">
         <v>112</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" t="s">
         <v>113</v>
-      </c>
-      <c r="D29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" t="s">
-        <v>114</v>
       </c>
       <c r="F29" t="s">
         <v>13</v>
@@ -2681,11 +2677,11 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>114</v>
+      </c>
+      <c r="C30" t="s">
         <v>115</v>
       </c>
-      <c r="C30" t="s">
-        <v>116</v>
-      </c>
       <c r="D30" t="s">
         <v>11</v>
       </c>
@@ -2693,7 +2689,7 @@
         <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G30" t="s">
         <v>19</v>
@@ -2702,7 +2698,7 @@
         <v>24</v>
       </c>
       <c r="I30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -2710,10 +2706,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
         <v>117</v>
-      </c>
-      <c r="C31" t="s">
-        <v>118</v>
       </c>
       <c r="D31" t="s">
         <v>11</v>
@@ -2739,22 +2735,22 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" t="s">
         <v>119</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
         <v>120</v>
       </c>
-      <c r="D32" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" t="s">
-        <v>121</v>
-      </c>
       <c r="G32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H32" t="s">
         <v>42</v>
@@ -2768,11 +2764,11 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
+        <v>121</v>
+      </c>
+      <c r="C33" t="s">
         <v>122</v>
       </c>
-      <c r="C33" t="s">
-        <v>123</v>
-      </c>
       <c r="D33" t="s">
         <v>11</v>
       </c>
@@ -2780,16 +2776,16 @@
         <v>12</v>
       </c>
       <c r="F33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G33" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H33" t="s">
         <v>42</v>
       </c>
       <c r="I33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:9">
@@ -2797,11 +2793,11 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
+        <v>123</v>
+      </c>
+      <c r="C34" t="s">
         <v>124</v>
       </c>
-      <c r="C34" t="s">
-        <v>125</v>
-      </c>
       <c r="D34" t="s">
         <v>11</v>
       </c>
@@ -2809,7 +2805,7 @@
         <v>12</v>
       </c>
       <c r="F34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G34" t="s">
         <v>32</v>
@@ -2818,7 +2814,7 @@
         <v>24</v>
       </c>
       <c r="I34" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="35" spans="1:9">
@@ -2826,28 +2822,28 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
+        <v>125</v>
+      </c>
+      <c r="C35" t="s">
         <v>126</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
         <v>127</v>
-      </c>
-      <c r="D35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" t="s">
-        <v>128</v>
       </c>
       <c r="G35" t="s">
         <v>24</v>
       </c>
       <c r="H35" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I35" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="36" spans="1:9">
@@ -2855,28 +2851,28 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
+        <v>128</v>
+      </c>
+      <c r="C36" t="s">
         <v>129</v>
       </c>
-      <c r="C36" t="s">
+      <c r="D36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" t="s">
         <v>130</v>
       </c>
-      <c r="D36" t="s">
-        <v>11</v>
-      </c>
-      <c r="E36" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" t="s">
-        <v>131</v>
-      </c>
       <c r="G36" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H36" t="s">
         <v>37</v>
       </c>
       <c r="I36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:9">
@@ -2884,11 +2880,11 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
+        <v>131</v>
+      </c>
+      <c r="C37" t="s">
         <v>132</v>
       </c>
-      <c r="C37" t="s">
-        <v>133</v>
-      </c>
       <c r="D37" t="s">
         <v>11</v>
       </c>
@@ -2896,13 +2892,13 @@
         <v>12</v>
       </c>
       <c r="F37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G37" t="s">
         <v>32</v>
       </c>
       <c r="H37" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I37" t="s">
         <v>20</v>
@@ -2913,19 +2909,19 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
+        <v>133</v>
+      </c>
+      <c r="C38" t="s">
         <v>134</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
         <v>135</v>
-      </c>
-      <c r="D38" t="s">
-        <v>11</v>
-      </c>
-      <c r="E38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" t="s">
-        <v>136</v>
       </c>
       <c r="G38" t="s">
         <v>19</v>
@@ -2942,10 +2938,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" t="s">
         <v>137</v>
-      </c>
-      <c r="C39" t="s">
-        <v>138</v>
       </c>
       <c r="D39" t="s">
         <v>11</v>
@@ -2963,7 +2959,7 @@
         <v>24</v>
       </c>
       <c r="I39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -2971,11 +2967,11 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
+        <v>139</v>
+      </c>
+      <c r="C40" t="s">
         <v>140</v>
       </c>
-      <c r="C40" t="s">
-        <v>141</v>
-      </c>
       <c r="D40" t="s">
         <v>11</v>
       </c>
@@ -2983,16 +2979,16 @@
         <v>12</v>
       </c>
       <c r="F40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G40" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="H40" t="s">
         <v>24</v>
       </c>
       <c r="I40" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -3000,10 +2996,10 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
+        <v>141</v>
+      </c>
+      <c r="C41" t="s">
         <v>142</v>
-      </c>
-      <c r="C41" t="s">
-        <v>143</v>
       </c>
       <c r="D41" t="s">
         <v>11</v>
@@ -3029,11 +3025,11 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" t="s">
         <v>144</v>
       </c>
-      <c r="C42" t="s">
-        <v>145</v>
-      </c>
       <c r="D42" t="s">
         <v>11</v>
       </c>
@@ -3041,16 +3037,16 @@
         <v>12</v>
       </c>
       <c r="F42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G42" t="s">
         <v>24</v>
       </c>
       <c r="H42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -3058,28 +3054,28 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
+        <v>145</v>
+      </c>
+      <c r="C43" t="s">
         <v>146</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
+        <v>11</v>
+      </c>
+      <c r="E43" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" t="s">
         <v>147</v>
       </c>
-      <c r="D43" t="s">
-        <v>11</v>
-      </c>
-      <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" t="s">
-        <v>148</v>
-      </c>
       <c r="G43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I43" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -3087,11 +3083,11 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" t="s">
         <v>149</v>
       </c>
-      <c r="C44" t="s">
-        <v>150</v>
-      </c>
       <c r="D44" t="s">
         <v>11</v>
       </c>
@@ -3099,7 +3095,7 @@
         <v>12</v>
       </c>
       <c r="F44" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G44" t="s">
         <v>18</v>
@@ -3116,10 +3112,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
+        <v>150</v>
+      </c>
+      <c r="C45" t="s">
         <v>151</v>
-      </c>
-      <c r="C45" t="s">
-        <v>152</v>
       </c>
       <c r="D45" t="s">
         <v>11</v>
@@ -3137,7 +3133,7 @@
         <v>24</v>
       </c>
       <c r="I45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -3145,11 +3141,11 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" t="s">
         <v>153</v>
       </c>
-      <c r="C46" t="s">
-        <v>154</v>
-      </c>
       <c r="D46" t="s">
         <v>11</v>
       </c>
@@ -3157,7 +3153,7 @@
         <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G46" t="s">
         <v>19</v>
@@ -3166,7 +3162,7 @@
         <v>18</v>
       </c>
       <c r="I46" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -3174,11 +3170,11 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
+        <v>154</v>
+      </c>
+      <c r="C47" t="s">
         <v>155</v>
       </c>
-      <c r="C47" t="s">
-        <v>156</v>
-      </c>
       <c r="D47" t="s">
         <v>11</v>
       </c>
@@ -3186,7 +3182,7 @@
         <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G47" t="s">
         <v>32</v>
@@ -3195,7 +3191,7 @@
         <v>18</v>
       </c>
       <c r="I47" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -3203,28 +3199,28 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" t="s">
         <v>157</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
+        <v>11</v>
+      </c>
+      <c r="E48" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" t="s">
         <v>158</v>
-      </c>
-      <c r="D48" t="s">
-        <v>11</v>
-      </c>
-      <c r="E48" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" t="s">
-        <v>159</v>
       </c>
       <c r="G48" t="s">
         <v>32</v>
       </c>
       <c r="H48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -3232,19 +3228,19 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>159</v>
+      </c>
+      <c r="C49" t="s">
         <v>160</v>
       </c>
-      <c r="C49" t="s">
-        <v>161</v>
-      </c>
       <c r="D49" t="s">
         <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F49" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G49" t="s">
         <v>37</v>
@@ -3253,7 +3249,7 @@
         <v>19</v>
       </c>
       <c r="I49" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -3261,19 +3257,19 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
+        <v>161</v>
+      </c>
+      <c r="C50" t="s">
         <v>162</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
         <v>163</v>
-      </c>
-      <c r="D50" t="s">
-        <v>11</v>
-      </c>
-      <c r="E50" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" t="s">
-        <v>164</v>
       </c>
       <c r="G50" t="s">
         <v>19</v>
@@ -3282,7 +3278,7 @@
         <v>24</v>
       </c>
       <c r="I50" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -3290,28 +3286,28 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C51" t="s">
         <v>165</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
+        <v>11</v>
+      </c>
+      <c r="E51" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
         <v>166</v>
       </c>
-      <c r="D51" t="s">
-        <v>11</v>
-      </c>
-      <c r="E51" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" t="s">
-        <v>167</v>
-      </c>
       <c r="G51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -3319,11 +3315,11 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
+        <v>167</v>
+      </c>
+      <c r="C52" t="s">
         <v>168</v>
       </c>
-      <c r="C52" t="s">
-        <v>169</v>
-      </c>
       <c r="D52" t="s">
         <v>11</v>
       </c>
@@ -3331,13 +3327,13 @@
         <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G52" t="s">
         <v>19</v>
       </c>
       <c r="H52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I52" t="s">
         <v>20</v>
@@ -3348,11 +3344,11 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
+        <v>169</v>
+      </c>
+      <c r="C53" t="s">
         <v>170</v>
       </c>
-      <c r="C53" t="s">
-        <v>171</v>
-      </c>
       <c r="D53" t="s">
         <v>11</v>
       </c>
@@ -3360,7 +3356,7 @@
         <v>12</v>
       </c>
       <c r="F53" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G53" t="s">
         <v>18</v>
@@ -3369,7 +3365,7 @@
         <v>25</v>
       </c>
       <c r="I53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -3377,22 +3373,22 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
+        <v>171</v>
+      </c>
+      <c r="C54" t="s">
         <v>172</v>
       </c>
-      <c r="C54" t="s">
-        <v>173</v>
-      </c>
       <c r="D54" t="s">
         <v>11</v>
       </c>
       <c r="E54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F54" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H54" t="s">
         <v>50</v>
@@ -3406,10 +3402,10 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
+        <v>173</v>
+      </c>
+      <c r="C55" t="s">
         <v>174</v>
-      </c>
-      <c r="C55" t="s">
-        <v>175</v>
       </c>
       <c r="D55" t="s">
         <v>11</v>
@@ -3427,7 +3423,7 @@
         <v>24</v>
       </c>
       <c r="I55" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -3435,28 +3431,28 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
+        <v>175</v>
+      </c>
+      <c r="C56" t="s">
         <v>176</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" t="s">
         <v>177</v>
       </c>
-      <c r="D56" t="s">
-        <v>11</v>
-      </c>
-      <c r="E56" t="s">
-        <v>12</v>
-      </c>
-      <c r="F56" t="s">
-        <v>178</v>
-      </c>
       <c r="G56" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H56" t="s">
         <v>24</v>
       </c>
       <c r="I56" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -3464,28 +3460,28 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
+        <v>178</v>
+      </c>
+      <c r="C57" t="s">
         <v>179</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
+        <v>11</v>
+      </c>
+      <c r="E57" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
         <v>180</v>
-      </c>
-      <c r="D57" t="s">
-        <v>11</v>
-      </c>
-      <c r="E57" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" t="s">
-        <v>181</v>
       </c>
       <c r="G57" t="s">
         <v>18</v>
       </c>
       <c r="H57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I57" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -3493,11 +3489,11 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
+        <v>181</v>
+      </c>
+      <c r="C58" t="s">
         <v>182</v>
       </c>
-      <c r="C58" t="s">
-        <v>183</v>
-      </c>
       <c r="D58" t="s">
         <v>11</v>
       </c>
@@ -3505,7 +3501,7 @@
         <v>12</v>
       </c>
       <c r="F58" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G58" t="s">
         <v>32</v>
@@ -3522,11 +3518,11 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
+        <v>183</v>
+      </c>
+      <c r="C59" t="s">
         <v>184</v>
       </c>
-      <c r="C59" t="s">
-        <v>185</v>
-      </c>
       <c r="D59" t="s">
         <v>11</v>
       </c>
@@ -3534,16 +3530,16 @@
         <v>12</v>
       </c>
       <c r="F59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G59" t="s">
         <v>24</v>
       </c>
       <c r="H59" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I59" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -3551,11 +3547,11 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
+        <v>185</v>
+      </c>
+      <c r="C60" t="s">
         <v>186</v>
       </c>
-      <c r="C60" t="s">
-        <v>187</v>
-      </c>
       <c r="D60" t="s">
         <v>11</v>
       </c>
@@ -3563,16 +3559,16 @@
         <v>12</v>
       </c>
       <c r="F60" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G60" t="s">
         <v>42</v>
       </c>
       <c r="H60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -3580,28 +3576,28 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
+        <v>187</v>
+      </c>
+      <c r="C61" t="s">
         <v>188</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" t="s">
         <v>189</v>
       </c>
-      <c r="D61" t="s">
-        <v>11</v>
-      </c>
-      <c r="E61" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61" t="s">
-        <v>190</v>
-      </c>
       <c r="G61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H61" t="s">
         <v>32</v>
       </c>
       <c r="I61" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -3609,10 +3605,10 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" t="s">
         <v>191</v>
-      </c>
-      <c r="C62" t="s">
-        <v>192</v>
       </c>
       <c r="D62" t="s">
         <v>11</v>
@@ -3630,7 +3626,7 @@
         <v>42</v>
       </c>
       <c r="I62" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -3638,11 +3634,11 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
+        <v>192</v>
+      </c>
+      <c r="C63" t="s">
         <v>193</v>
       </c>
-      <c r="C63" t="s">
-        <v>194</v>
-      </c>
       <c r="D63" t="s">
         <v>11</v>
       </c>
@@ -3650,16 +3646,16 @@
         <v>12</v>
       </c>
       <c r="F63" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G63" t="s">
         <v>32</v>
       </c>
       <c r="H63" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I63" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -3667,11 +3663,11 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" t="s">
         <v>195</v>
       </c>
-      <c r="C64" t="s">
-        <v>196</v>
-      </c>
       <c r="D64" t="s">
         <v>11</v>
       </c>
@@ -3679,16 +3675,16 @@
         <v>12</v>
       </c>
       <c r="F64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G64" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I64" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="65" spans="1:9">
@@ -3696,28 +3692,28 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
+        <v>196</v>
+      </c>
+      <c r="C65" t="s">
         <v>197</v>
       </c>
-      <c r="C65" t="s">
-        <v>198</v>
-      </c>
       <c r="D65" t="s">
         <v>11</v>
       </c>
       <c r="E65" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G65" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I65" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="66" spans="1:9">
@@ -3725,10 +3721,10 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
+        <v>198</v>
+      </c>
+      <c r="C66" t="s">
         <v>199</v>
-      </c>
-      <c r="C66" t="s">
-        <v>200</v>
       </c>
       <c r="D66" t="s">
         <v>11</v>
@@ -3743,10 +3739,10 @@
         <v>32</v>
       </c>
       <c r="H66" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I66" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:9">
@@ -3754,11 +3750,11 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
+        <v>200</v>
+      </c>
+      <c r="C67" t="s">
         <v>201</v>
       </c>
-      <c r="C67" t="s">
-        <v>202</v>
-      </c>
       <c r="D67" t="s">
         <v>11</v>
       </c>
@@ -3766,7 +3762,7 @@
         <v>12</v>
       </c>
       <c r="F67" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G67" t="s">
         <v>42</v>
@@ -3775,7 +3771,7 @@
         <v>42</v>
       </c>
       <c r="I67" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="68" spans="1:9">
@@ -3783,10 +3779,10 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
+        <v>202</v>
+      </c>
+      <c r="C68" t="s">
         <v>203</v>
-      </c>
-      <c r="C68" t="s">
-        <v>204</v>
       </c>
       <c r="D68" t="s">
         <v>11</v>
@@ -3804,7 +3800,7 @@
         <v>18</v>
       </c>
       <c r="I68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="69" spans="1:9">
@@ -3812,11 +3808,11 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
+        <v>204</v>
+      </c>
+      <c r="C69" t="s">
         <v>205</v>
       </c>
-      <c r="C69" t="s">
-        <v>206</v>
-      </c>
       <c r="D69" t="s">
         <v>11</v>
       </c>
@@ -3824,7 +3820,7 @@
         <v>12</v>
       </c>
       <c r="F69" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G69" t="s">
         <v>19</v>
@@ -3833,7 +3829,7 @@
         <v>24</v>
       </c>
       <c r="I69" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="70" spans="1:9">
@@ -3841,10 +3837,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
+        <v>206</v>
+      </c>
+      <c r="C70" t="s">
         <v>207</v>
-      </c>
-      <c r="C70" t="s">
-        <v>208</v>
       </c>
       <c r="D70" t="s">
         <v>11</v>
@@ -3856,7 +3852,7 @@
         <v>26</v>
       </c>
       <c r="G70" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H70" t="s">
         <v>42</v>
@@ -3870,11 +3866,11 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
+        <v>208</v>
+      </c>
+      <c r="C71" t="s">
         <v>209</v>
       </c>
-      <c r="C71" t="s">
-        <v>210</v>
-      </c>
       <c r="D71" t="s">
         <v>11</v>
       </c>
@@ -3882,21 +3878,21 @@
         <v>12</v>
       </c>
       <c r="F71" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ wanghuaijin/wanghuaijin.github.io@e417e31bf6067b18695a7361705942a81e9d1752 🚀
</commit_message>
<xml_diff>
--- a/assets/numDEs/status/evaluation.xlsx
+++ b/assets/numDEs/status/evaluation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="149">
   <si>
     <t>序号</t>
   </si>
@@ -44,18 +44,6 @@
     <t>专业名称</t>
   </si>
   <si>
-    <t>平时作业分数</t>
-  </si>
-  <si>
-    <t>上机报告1</t>
-  </si>
-  <si>
-    <t>上机报告2</t>
-  </si>
-  <si>
-    <t>出勤率</t>
-  </si>
-  <si>
     <t>19020182203624</t>
   </si>
   <si>
@@ -68,129 +56,60 @@
     <t>信息与计算科学</t>
   </si>
   <si>
-    <t>0%</t>
-  </si>
-  <si>
-    <t>Ｏ</t>
-  </si>
-  <si>
     <t>19020202200624</t>
   </si>
   <si>
     <t>杜雨晴</t>
   </si>
   <si>
-    <t>61%</t>
-  </si>
-  <si>
-    <t>70%</t>
-  </si>
-  <si>
-    <t>50%</t>
-  </si>
-  <si>
-    <t>97%</t>
-  </si>
-  <si>
     <t>19020202202514</t>
   </si>
   <si>
     <t>牛雅茹</t>
   </si>
   <si>
-    <t>47%</t>
-  </si>
-  <si>
-    <t>80%</t>
-  </si>
-  <si>
-    <t>30%</t>
-  </si>
-  <si>
-    <t>89%</t>
-  </si>
-  <si>
     <t>19020202202528</t>
   </si>
   <si>
     <t>张世豪</t>
   </si>
   <si>
-    <t>42%</t>
-  </si>
-  <si>
     <t>19020202204352</t>
   </si>
   <si>
     <t>郭紫熙</t>
   </si>
   <si>
-    <t>60%</t>
-  </si>
-  <si>
-    <t>78%</t>
-  </si>
-  <si>
     <t>19020202204366</t>
   </si>
   <si>
     <t>邢炳萱</t>
   </si>
   <si>
-    <t>34%</t>
-  </si>
-  <si>
-    <t>40%</t>
-  </si>
-  <si>
-    <t>8%</t>
-  </si>
-  <si>
     <t>19020212203411</t>
   </si>
   <si>
     <t>陈宇润</t>
   </si>
   <si>
-    <t>46%</t>
-  </si>
-  <si>
-    <t>90%</t>
-  </si>
-  <si>
-    <t>83%</t>
-  </si>
-  <si>
     <t>19020212203415</t>
   </si>
   <si>
     <t>戴子恒</t>
   </si>
   <si>
-    <t>54%</t>
-  </si>
-  <si>
     <t>19020212203422</t>
   </si>
   <si>
     <t>韩双御</t>
   </si>
   <si>
-    <t>28%</t>
-  </si>
-  <si>
-    <t>75%</t>
-  </si>
-  <si>
     <t>19020212203431</t>
   </si>
   <si>
     <t>黄学敏</t>
   </si>
   <si>
-    <t>49%</t>
-  </si>
-  <si>
     <t>19020212203434</t>
   </si>
   <si>
@@ -203,63 +122,30 @@
     <t>刘清华</t>
   </si>
   <si>
-    <t>69%</t>
-  </si>
-  <si>
-    <t>65%</t>
-  </si>
-  <si>
-    <t>67%</t>
-  </si>
-  <si>
     <t>19020212203455</t>
   </si>
   <si>
     <t>刘铮武</t>
   </si>
   <si>
-    <t>44%</t>
-  </si>
-  <si>
-    <t>72%</t>
-  </si>
-  <si>
     <t>19020212203466</t>
   </si>
   <si>
     <t>邵译萱</t>
   </si>
   <si>
-    <t>20%</t>
-  </si>
-  <si>
-    <t>92%</t>
-  </si>
-  <si>
     <t>19020212203470</t>
   </si>
   <si>
     <t>田加林</t>
   </si>
   <si>
-    <t>59%</t>
-  </si>
-  <si>
-    <t>100%</t>
-  </si>
-  <si>
     <t>19020212203473</t>
   </si>
   <si>
     <t>王清林</t>
   </si>
   <si>
-    <t>63%</t>
-  </si>
-  <si>
-    <t>95%</t>
-  </si>
-  <si>
     <t>19020212203494</t>
   </si>
   <si>
@@ -272,81 +158,48 @@
     <t>杨雨涵</t>
   </si>
   <si>
-    <t>45%</t>
-  </si>
-  <si>
-    <t>64%</t>
-  </si>
-  <si>
     <t>19020212203509</t>
   </si>
   <si>
     <t>张永琦</t>
   </si>
   <si>
-    <t>16%</t>
-  </si>
-  <si>
     <t>19020212203510</t>
   </si>
   <si>
     <t>赵庆尧</t>
   </si>
   <si>
-    <t>66%</t>
-  </si>
-  <si>
     <t>19020222202291</t>
   </si>
   <si>
     <t>陈珂楠</t>
   </si>
   <si>
-    <t>86%</t>
-  </si>
-  <si>
     <t>19020222202292</t>
   </si>
   <si>
     <t>傅凌瑶</t>
   </si>
   <si>
-    <t>87%</t>
-  </si>
-  <si>
     <t>19020222202295</t>
   </si>
   <si>
     <t>李清星</t>
   </si>
   <si>
-    <t>55%</t>
-  </si>
-  <si>
     <t>19020222202296</t>
   </si>
   <si>
     <t>李欣然</t>
   </si>
   <si>
-    <t>11%</t>
-  </si>
-  <si>
-    <t>85%</t>
-  </si>
-  <si>
     <t>20420202201837</t>
   </si>
   <si>
     <t>徐清源</t>
   </si>
   <si>
-    <t>68%</t>
-  </si>
-  <si>
-    <t>81%</t>
-  </si>
-  <si>
     <t>25120212202184</t>
   </si>
   <si>
@@ -359,9 +212,6 @@
     <t>庄博诚</t>
   </si>
   <si>
-    <t>98%</t>
-  </si>
-  <si>
     <t>25120222201341</t>
   </si>
   <si>
@@ -389,9 +239,6 @@
     <t>程禹</t>
   </si>
   <si>
-    <t>93%</t>
-  </si>
-  <si>
     <t>37520222204672</t>
   </si>
   <si>
@@ -410,18 +257,12 @@
     <t>陈鸿达</t>
   </si>
   <si>
-    <t>82%</t>
-  </si>
-  <si>
     <t>37720222204905</t>
   </si>
   <si>
     <t>陈筱锋</t>
   </si>
   <si>
-    <t>58%</t>
-  </si>
-  <si>
     <t>37720222204913</t>
   </si>
   <si>
@@ -434,18 +275,12 @@
     <t>高源</t>
   </si>
   <si>
-    <t>74%</t>
-  </si>
-  <si>
     <t>37720222204939</t>
   </si>
   <si>
     <t>连传瀚</t>
   </si>
   <si>
-    <t>94%</t>
-  </si>
-  <si>
     <t>37720222204941</t>
   </si>
   <si>
@@ -470,9 +305,6 @@
     <t>吕阳</t>
   </si>
   <si>
-    <t>88%</t>
-  </si>
-  <si>
     <t>37720222204966</t>
   </si>
   <si>
@@ -503,9 +335,6 @@
     <t>张庄辉</t>
   </si>
   <si>
-    <t>84%</t>
-  </si>
-  <si>
     <t>37720222204990</t>
   </si>
   <si>
@@ -518,18 +347,12 @@
     <t>周家辉</t>
   </si>
   <si>
-    <t>71%</t>
-  </si>
-  <si>
     <t>37720222204998</t>
   </si>
   <si>
     <t>卜於锴</t>
   </si>
   <si>
-    <t>91%</t>
-  </si>
-  <si>
     <t>37720222204999</t>
   </si>
   <si>
@@ -560,18 +383,12 @@
     <t>何锦弘</t>
   </si>
   <si>
-    <t>73%</t>
-  </si>
-  <si>
     <t>37720222205021</t>
   </si>
   <si>
     <t>洪怡洁</t>
   </si>
   <si>
-    <t>96%</t>
-  </si>
-  <si>
     <t>37720222205026</t>
   </si>
   <si>
@@ -594,9 +411,6 @@
   </si>
   <si>
     <t>宋锐扬</t>
-  </si>
-  <si>
-    <t>79%</t>
   </si>
   <si>
     <t>37720222205078</t>
@@ -1813,25 +1627,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A40" sqref="$A40:$XFD40"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.3984375" customWidth="1"/>
-    <col min="4" max="4" width="18.359375" customWidth="1"/>
-    <col min="5" max="5" width="14.8359375" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="8" width="6.7109375" customWidth="1"/>
-    <col min="9" max="9" width="5.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.7109375" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1847,2052 +1658,1200 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>65</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>66</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>23</v>
-      </c>
-      <c r="G15" t="s">
-        <v>67</v>
-      </c>
-      <c r="H15" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>70</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" t="s">
-        <v>32</v>
-      </c>
-      <c r="H16" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>73</v>
+        <v>37</v>
       </c>
       <c r="C17" t="s">
-        <v>74</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" t="s">
-        <v>76</v>
-      </c>
-      <c r="I17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>77</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" t="s">
-        <v>81</v>
-      </c>
-      <c r="G19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" t="s">
-        <v>81</v>
-      </c>
-      <c r="I19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>12</v>
-      </c>
-      <c r="F20" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" t="s">
-        <v>32</v>
-      </c>
-      <c r="H20" t="s">
-        <v>18</v>
-      </c>
-      <c r="I20" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" t="s">
-        <v>32</v>
-      </c>
-      <c r="I21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>89</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>12</v>
-      </c>
-      <c r="F22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>50</v>
       </c>
       <c r="D23" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>12</v>
-      </c>
-      <c r="F23" t="s">
-        <v>94</v>
-      </c>
-      <c r="G23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H23" t="s">
-        <v>42</v>
-      </c>
-      <c r="I23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>95</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
       <c r="D24" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" t="s">
-        <v>97</v>
-      </c>
-      <c r="G24" t="s">
-        <v>19</v>
-      </c>
-      <c r="H24" t="s">
-        <v>24</v>
-      </c>
-      <c r="I24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>99</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
-      </c>
-      <c r="F25" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" t="s">
-        <v>50</v>
-      </c>
-      <c r="H25" t="s">
-        <v>101</v>
-      </c>
-      <c r="I25" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>102</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>56</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>12</v>
-      </c>
-      <c r="F26" t="s">
-        <v>104</v>
-      </c>
-      <c r="G26" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" t="s">
-        <v>72</v>
-      </c>
-      <c r="I26" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" t="s">
-        <v>72</v>
-      </c>
-      <c r="I27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>59</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" t="s">
-        <v>110</v>
-      </c>
-      <c r="G28" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" t="s">
-        <v>72</v>
-      </c>
-      <c r="I28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="D29" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>113</v>
-      </c>
-      <c r="F29" t="s">
-        <v>13</v>
-      </c>
-      <c r="G29" t="s">
-        <v>14</v>
-      </c>
-      <c r="H29" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="C30" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="D30" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G30" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>12</v>
-      </c>
-      <c r="F31" t="s">
-        <v>50</v>
-      </c>
-      <c r="G31" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" t="s">
-        <v>32</v>
-      </c>
-      <c r="I31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" t="s">
-        <v>120</v>
-      </c>
-      <c r="G32" t="s">
-        <v>59</v>
-      </c>
-      <c r="H32" t="s">
-        <v>42</v>
-      </c>
-      <c r="I32" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="C33" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G33" t="s">
-        <v>24</v>
-      </c>
-      <c r="H33" t="s">
-        <v>42</v>
-      </c>
-      <c r="I33" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="D34" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>12</v>
-      </c>
-      <c r="F34" t="s">
-        <v>94</v>
-      </c>
-      <c r="G34" t="s">
-        <v>32</v>
-      </c>
-      <c r="H34" t="s">
-        <v>24</v>
-      </c>
-      <c r="I34" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="C35" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E35" t="s">
-        <v>12</v>
-      </c>
-      <c r="F35" t="s">
-        <v>127</v>
-      </c>
-      <c r="G35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H35" t="s">
-        <v>101</v>
-      </c>
-      <c r="I35" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>128</v>
+        <v>76</v>
       </c>
       <c r="C36" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E36" t="s">
-        <v>113</v>
-      </c>
-      <c r="F36" t="s">
-        <v>130</v>
-      </c>
-      <c r="G36" t="s">
-        <v>67</v>
-      </c>
-      <c r="H36" t="s">
-        <v>37</v>
-      </c>
-      <c r="I36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>78</v>
       </c>
       <c r="C37" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="D37" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E37" t="s">
-        <v>12</v>
-      </c>
-      <c r="F37" t="s">
-        <v>71</v>
-      </c>
-      <c r="G37" t="s">
-        <v>32</v>
-      </c>
-      <c r="H37" t="s">
-        <v>101</v>
-      </c>
-      <c r="I37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>133</v>
+        <v>80</v>
       </c>
       <c r="C38" t="s">
-        <v>134</v>
+        <v>81</v>
       </c>
       <c r="D38" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E38" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" t="s">
-        <v>135</v>
-      </c>
-      <c r="G38" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" t="s">
-        <v>32</v>
-      </c>
-      <c r="I38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>82</v>
       </c>
       <c r="C39" t="s">
-        <v>137</v>
+        <v>83</v>
       </c>
       <c r="D39" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E39" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" t="s">
-        <v>17</v>
-      </c>
-      <c r="G39" t="s">
-        <v>24</v>
-      </c>
-      <c r="H39" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>139</v>
+        <v>84</v>
       </c>
       <c r="C40" t="s">
-        <v>140</v>
+        <v>85</v>
       </c>
       <c r="D40" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E40" t="s">
-        <v>12</v>
-      </c>
-      <c r="F40" t="s">
-        <v>94</v>
-      </c>
-      <c r="G40" t="s">
-        <v>32</v>
-      </c>
-      <c r="H40" t="s">
-        <v>24</v>
-      </c>
-      <c r="I40" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>141</v>
+        <v>86</v>
       </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>87</v>
       </c>
       <c r="D41" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>12</v>
-      </c>
-      <c r="F41" t="s">
-        <v>24</v>
-      </c>
-      <c r="G41" t="s">
-        <v>32</v>
-      </c>
-      <c r="H41" t="s">
-        <v>42</v>
-      </c>
-      <c r="I41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>143</v>
+        <v>88</v>
       </c>
       <c r="C42" t="s">
-        <v>144</v>
+        <v>89</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E42" t="s">
-        <v>12</v>
-      </c>
-      <c r="F42" t="s">
-        <v>94</v>
-      </c>
-      <c r="G42" t="s">
-        <v>24</v>
-      </c>
-      <c r="H42" t="s">
-        <v>72</v>
-      </c>
-      <c r="I42" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>145</v>
+        <v>90</v>
       </c>
       <c r="C43" t="s">
-        <v>146</v>
+        <v>91</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>12</v>
-      </c>
-      <c r="F43" t="s">
-        <v>147</v>
-      </c>
-      <c r="G43" t="s">
-        <v>72</v>
-      </c>
-      <c r="H43" t="s">
-        <v>72</v>
-      </c>
-      <c r="I43" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>148</v>
+        <v>92</v>
       </c>
       <c r="C44" t="s">
-        <v>149</v>
+        <v>93</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>12</v>
-      </c>
-      <c r="F44" t="s">
-        <v>127</v>
-      </c>
-      <c r="G44" t="s">
-        <v>18</v>
-      </c>
-      <c r="H44" t="s">
-        <v>24</v>
-      </c>
-      <c r="I44" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>94</v>
       </c>
       <c r="C45" t="s">
-        <v>151</v>
+        <v>95</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>12</v>
-      </c>
-      <c r="F45" t="s">
-        <v>42</v>
-      </c>
-      <c r="G45" t="s">
-        <v>32</v>
-      </c>
-      <c r="H45" t="s">
-        <v>24</v>
-      </c>
-      <c r="I45" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>152</v>
+        <v>96</v>
       </c>
       <c r="C46" t="s">
-        <v>153</v>
+        <v>97</v>
       </c>
       <c r="D46" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E46" t="s">
-        <v>12</v>
-      </c>
-      <c r="F46" t="s">
-        <v>105</v>
-      </c>
-      <c r="G46" t="s">
-        <v>19</v>
-      </c>
-      <c r="H46" t="s">
-        <v>18</v>
-      </c>
-      <c r="I46" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>154</v>
+        <v>98</v>
       </c>
       <c r="C47" t="s">
-        <v>155</v>
+        <v>99</v>
       </c>
       <c r="D47" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47" t="s">
-        <v>94</v>
-      </c>
-      <c r="G47" t="s">
-        <v>32</v>
-      </c>
-      <c r="H47" t="s">
-        <v>18</v>
-      </c>
-      <c r="I47" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>156</v>
+        <v>100</v>
       </c>
       <c r="C48" t="s">
-        <v>157</v>
+        <v>101</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>12</v>
-      </c>
-      <c r="F48" t="s">
-        <v>158</v>
-      </c>
-      <c r="G48" t="s">
-        <v>32</v>
-      </c>
-      <c r="H48" t="s">
-        <v>72</v>
-      </c>
-      <c r="I48" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>159</v>
+        <v>102</v>
       </c>
       <c r="C49" t="s">
-        <v>160</v>
+        <v>103</v>
       </c>
       <c r="D49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E49" t="s">
-        <v>113</v>
-      </c>
-      <c r="F49" t="s">
-        <v>147</v>
-      </c>
-      <c r="G49" t="s">
-        <v>37</v>
-      </c>
-      <c r="H49" t="s">
-        <v>19</v>
-      </c>
-      <c r="I49" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="C50" t="s">
-        <v>162</v>
+        <v>105</v>
       </c>
       <c r="D50" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E50" t="s">
-        <v>12</v>
-      </c>
-      <c r="F50" t="s">
-        <v>163</v>
-      </c>
-      <c r="G50" t="s">
-        <v>19</v>
-      </c>
-      <c r="H50" t="s">
-        <v>24</v>
-      </c>
-      <c r="I50" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>164</v>
+        <v>106</v>
       </c>
       <c r="C51" t="s">
-        <v>165</v>
+        <v>107</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E51" t="s">
-        <v>12</v>
-      </c>
-      <c r="F51" t="s">
-        <v>166</v>
-      </c>
-      <c r="G51" t="s">
-        <v>59</v>
-      </c>
-      <c r="H51" t="s">
-        <v>72</v>
-      </c>
-      <c r="I51" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>167</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>168</v>
+        <v>109</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E52" t="s">
-        <v>12</v>
-      </c>
-      <c r="F52" t="s">
-        <v>94</v>
-      </c>
-      <c r="G52" t="s">
-        <v>19</v>
-      </c>
-      <c r="H52" t="s">
-        <v>101</v>
-      </c>
-      <c r="I52" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>169</v>
+        <v>110</v>
       </c>
       <c r="C53" t="s">
-        <v>170</v>
+        <v>111</v>
       </c>
       <c r="D53" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E53" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" t="s">
-        <v>91</v>
-      </c>
-      <c r="G53" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53" t="s">
-        <v>25</v>
-      </c>
-      <c r="I53" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>112</v>
       </c>
       <c r="C54" t="s">
-        <v>172</v>
+        <v>113</v>
       </c>
       <c r="D54" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E54" t="s">
-        <v>113</v>
-      </c>
-      <c r="F54" t="s">
-        <v>97</v>
-      </c>
-      <c r="G54" t="s">
-        <v>59</v>
-      </c>
-      <c r="H54" t="s">
-        <v>50</v>
-      </c>
-      <c r="I54" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>173</v>
+        <v>114</v>
       </c>
       <c r="C55" t="s">
-        <v>174</v>
+        <v>115</v>
       </c>
       <c r="D55" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E55" t="s">
-        <v>12</v>
-      </c>
-      <c r="F55" t="s">
-        <v>26</v>
-      </c>
-      <c r="G55" t="s">
-        <v>24</v>
-      </c>
-      <c r="H55" t="s">
-        <v>24</v>
-      </c>
-      <c r="I55" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>175</v>
+        <v>116</v>
       </c>
       <c r="C56" t="s">
-        <v>176</v>
+        <v>117</v>
       </c>
       <c r="D56" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E56" t="s">
-        <v>12</v>
-      </c>
-      <c r="F56" t="s">
-        <v>177</v>
-      </c>
-      <c r="G56" t="s">
-        <v>101</v>
-      </c>
-      <c r="H56" t="s">
-        <v>24</v>
-      </c>
-      <c r="I56" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>178</v>
+        <v>118</v>
       </c>
       <c r="C57" t="s">
-        <v>179</v>
+        <v>119</v>
       </c>
       <c r="D57" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E57" t="s">
-        <v>12</v>
-      </c>
-      <c r="F57" t="s">
-        <v>180</v>
-      </c>
-      <c r="G57" t="s">
-        <v>18</v>
-      </c>
-      <c r="H57" t="s">
-        <v>72</v>
-      </c>
-      <c r="I57" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>181</v>
+        <v>120</v>
       </c>
       <c r="C58" t="s">
-        <v>182</v>
+        <v>121</v>
       </c>
       <c r="D58" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E58" t="s">
-        <v>12</v>
-      </c>
-      <c r="F58" t="s">
-        <v>130</v>
-      </c>
-      <c r="G58" t="s">
-        <v>32</v>
-      </c>
-      <c r="H58" t="s">
-        <v>42</v>
-      </c>
-      <c r="I58" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>183</v>
+        <v>122</v>
       </c>
       <c r="C59" t="s">
-        <v>184</v>
+        <v>123</v>
       </c>
       <c r="D59" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E59" t="s">
-        <v>12</v>
-      </c>
-      <c r="F59" t="s">
-        <v>147</v>
-      </c>
-      <c r="G59" t="s">
-        <v>24</v>
-      </c>
-      <c r="H59" t="s">
-        <v>101</v>
-      </c>
-      <c r="I59" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>185</v>
+        <v>124</v>
       </c>
       <c r="C60" t="s">
-        <v>186</v>
+        <v>125</v>
       </c>
       <c r="D60" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>12</v>
-      </c>
-      <c r="F60" t="s">
-        <v>68</v>
-      </c>
-      <c r="G60" t="s">
-        <v>42</v>
-      </c>
-      <c r="H60" t="s">
-        <v>72</v>
-      </c>
-      <c r="I60" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="C61" t="s">
-        <v>188</v>
+        <v>127</v>
       </c>
       <c r="D61" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E61" t="s">
-        <v>12</v>
-      </c>
-      <c r="F61" t="s">
-        <v>189</v>
-      </c>
-      <c r="G61" t="s">
-        <v>59</v>
-      </c>
-      <c r="H61" t="s">
-        <v>32</v>
-      </c>
-      <c r="I61" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>190</v>
+        <v>128</v>
       </c>
       <c r="C62" t="s">
-        <v>191</v>
+        <v>129</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E62" t="s">
-        <v>12</v>
-      </c>
-      <c r="F62" t="s">
-        <v>26</v>
-      </c>
-      <c r="G62" t="s">
-        <v>32</v>
-      </c>
-      <c r="H62" t="s">
-        <v>42</v>
-      </c>
-      <c r="I62" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>192</v>
+        <v>130</v>
       </c>
       <c r="C63" t="s">
-        <v>193</v>
+        <v>131</v>
       </c>
       <c r="D63" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E63" t="s">
-        <v>12</v>
-      </c>
-      <c r="F63" t="s">
-        <v>58</v>
-      </c>
-      <c r="G63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H63" t="s">
-        <v>72</v>
-      </c>
-      <c r="I63" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>194</v>
+        <v>132</v>
       </c>
       <c r="C64" t="s">
-        <v>195</v>
+        <v>133</v>
       </c>
       <c r="D64" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>12</v>
-      </c>
-      <c r="F64" t="s">
-        <v>120</v>
-      </c>
-      <c r="G64" t="s">
-        <v>59</v>
-      </c>
-      <c r="H64" t="s">
-        <v>72</v>
-      </c>
-      <c r="I64" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>196</v>
+        <v>134</v>
       </c>
       <c r="C65" t="s">
-        <v>197</v>
+        <v>135</v>
       </c>
       <c r="D65" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E65" t="s">
-        <v>113</v>
-      </c>
-      <c r="F65" t="s">
-        <v>120</v>
-      </c>
-      <c r="G65" t="s">
-        <v>76</v>
-      </c>
-      <c r="H65" t="s">
-        <v>72</v>
-      </c>
-      <c r="I65" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>198</v>
+        <v>136</v>
       </c>
       <c r="C66" t="s">
-        <v>199</v>
+        <v>137</v>
       </c>
       <c r="D66" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E66" t="s">
-        <v>12</v>
-      </c>
-      <c r="F66" t="s">
-        <v>26</v>
-      </c>
-      <c r="G66" t="s">
-        <v>32</v>
-      </c>
-      <c r="H66" t="s">
-        <v>101</v>
-      </c>
-      <c r="I66" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>200</v>
+        <v>138</v>
       </c>
       <c r="C67" t="s">
-        <v>201</v>
+        <v>139</v>
       </c>
       <c r="D67" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E67" t="s">
-        <v>12</v>
-      </c>
-      <c r="F67" t="s">
-        <v>166</v>
-      </c>
-      <c r="G67" t="s">
-        <v>42</v>
-      </c>
-      <c r="H67" t="s">
-        <v>42</v>
-      </c>
-      <c r="I67" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>202</v>
+        <v>140</v>
       </c>
       <c r="C68" t="s">
-        <v>203</v>
+        <v>141</v>
       </c>
       <c r="D68" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>12</v>
-      </c>
-      <c r="F68" t="s">
-        <v>50</v>
-      </c>
-      <c r="G68" t="s">
-        <v>32</v>
-      </c>
-      <c r="H68" t="s">
-        <v>18</v>
-      </c>
-      <c r="I68" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>204</v>
+        <v>142</v>
       </c>
       <c r="C69" t="s">
-        <v>205</v>
+        <v>143</v>
       </c>
       <c r="D69" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E69" t="s">
-        <v>12</v>
-      </c>
-      <c r="F69" t="s">
-        <v>68</v>
-      </c>
-      <c r="G69" t="s">
-        <v>19</v>
-      </c>
-      <c r="H69" t="s">
-        <v>24</v>
-      </c>
-      <c r="I69" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>206</v>
+        <v>144</v>
       </c>
       <c r="C70" t="s">
-        <v>207</v>
+        <v>145</v>
       </c>
       <c r="D70" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E70" t="s">
-        <v>12</v>
-      </c>
-      <c r="F70" t="s">
-        <v>26</v>
-      </c>
-      <c r="G70" t="s">
-        <v>59</v>
-      </c>
-      <c r="H70" t="s">
-        <v>42</v>
-      </c>
-      <c r="I70" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>208</v>
+        <v>146</v>
       </c>
       <c r="C71" t="s">
-        <v>209</v>
+        <v>147</v>
       </c>
       <c r="D71" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E71" t="s">
-        <v>12</v>
-      </c>
-      <c r="F71" t="s">
-        <v>76</v>
-      </c>
-      <c r="G71" t="s">
-        <v>72</v>
-      </c>
-      <c r="H71" t="s">
-        <v>72</v>
-      </c>
-      <c r="I71" t="s">
-        <v>72</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" t="s">
-        <v>210</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deploying to gh-pages from @ wanghuaijin/wanghuaijin.github.io@0af1958b30b8ea8d23044e7397dbf357a376572d 🚀
</commit_message>
<xml_diff>
--- a/assets/numDEs/status/evaluation.xlsx
+++ b/assets/numDEs/status/evaluation.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="210">
   <si>
     <t>序号</t>
   </si>
@@ -44,6 +44,18 @@
     <t>专业名称</t>
   </si>
   <si>
+    <t>平时作业分数</t>
+  </si>
+  <si>
+    <t>上机报告1</t>
+  </si>
+  <si>
+    <t>上机报告2</t>
+  </si>
+  <si>
+    <t>出勤率</t>
+  </si>
+  <si>
     <t>19020182203624</t>
   </si>
   <si>
@@ -56,60 +68,129 @@
     <t>信息与计算科学</t>
   </si>
   <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>Ｏ</t>
+  </si>
+  <si>
     <t>19020202200624</t>
   </si>
   <si>
     <t>杜雨晴</t>
   </si>
   <si>
+    <t>61%</t>
+  </si>
+  <si>
+    <t>70%</t>
+  </si>
+  <si>
+    <t>50%</t>
+  </si>
+  <si>
+    <t>97%</t>
+  </si>
+  <si>
     <t>19020202202514</t>
   </si>
   <si>
     <t>牛雅茹</t>
   </si>
   <si>
+    <t>47%</t>
+  </si>
+  <si>
+    <t>80%</t>
+  </si>
+  <si>
+    <t>30%</t>
+  </si>
+  <si>
+    <t>89%</t>
+  </si>
+  <si>
     <t>19020202202528</t>
   </si>
   <si>
     <t>张世豪</t>
   </si>
   <si>
+    <t>42%</t>
+  </si>
+  <si>
     <t>19020202204352</t>
   </si>
   <si>
     <t>郭紫熙</t>
   </si>
   <si>
+    <t>60%</t>
+  </si>
+  <si>
+    <t>78%</t>
+  </si>
+  <si>
     <t>19020202204366</t>
   </si>
   <si>
     <t>邢炳萱</t>
   </si>
   <si>
+    <t>14%</t>
+  </si>
+  <si>
+    <t>40%</t>
+  </si>
+  <si>
+    <t>8%</t>
+  </si>
+  <si>
     <t>19020212203411</t>
   </si>
   <si>
     <t>陈宇润</t>
   </si>
   <si>
+    <t>46%</t>
+  </si>
+  <si>
+    <t>90%</t>
+  </si>
+  <si>
+    <t>83%</t>
+  </si>
+  <si>
     <t>19020212203415</t>
   </si>
   <si>
     <t>戴子恒</t>
   </si>
   <si>
+    <t>54%</t>
+  </si>
+  <si>
     <t>19020212203422</t>
   </si>
   <si>
     <t>韩双御</t>
   </si>
   <si>
+    <t>28%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
     <t>19020212203431</t>
   </si>
   <si>
     <t>黄学敏</t>
   </si>
   <si>
+    <t>49%</t>
+  </si>
+  <si>
     <t>19020212203434</t>
   </si>
   <si>
@@ -122,30 +203,63 @@
     <t>刘清华</t>
   </si>
   <si>
+    <t>58%</t>
+  </si>
+  <si>
+    <t>65%</t>
+  </si>
+  <si>
+    <t>67%</t>
+  </si>
+  <si>
     <t>19020212203455</t>
   </si>
   <si>
     <t>刘铮武</t>
   </si>
   <si>
+    <t>44%</t>
+  </si>
+  <si>
+    <t>72%</t>
+  </si>
+  <si>
     <t>19020212203466</t>
   </si>
   <si>
     <t>邵译萱</t>
   </si>
   <si>
+    <t>20%</t>
+  </si>
+  <si>
+    <t>92%</t>
+  </si>
+  <si>
     <t>19020212203470</t>
   </si>
   <si>
     <t>田加林</t>
   </si>
   <si>
+    <t>59%</t>
+  </si>
+  <si>
+    <t>100%</t>
+  </si>
+  <si>
     <t>19020212203473</t>
   </si>
   <si>
     <t>王清林</t>
   </si>
   <si>
+    <t>63%</t>
+  </si>
+  <si>
+    <t>95%</t>
+  </si>
+  <si>
     <t>19020212203494</t>
   </si>
   <si>
@@ -158,12 +272,24 @@
     <t>杨雨涵</t>
   </si>
   <si>
+    <t>37%</t>
+  </si>
+  <si>
+    <t>45%</t>
+  </si>
+  <si>
+    <t>64%</t>
+  </si>
+  <si>
     <t>19020212203509</t>
   </si>
   <si>
     <t>张永琦</t>
   </si>
   <si>
+    <t>33%</t>
+  </si>
+  <si>
     <t>19020212203510</t>
   </si>
   <si>
@@ -176,30 +302,54 @@
     <t>陈珂楠</t>
   </si>
   <si>
+    <t>86%</t>
+  </si>
+  <si>
     <t>19020222202292</t>
   </si>
   <si>
     <t>傅凌瑶</t>
   </si>
   <si>
+    <t>87%</t>
+  </si>
+  <si>
     <t>19020222202295</t>
   </si>
   <si>
     <t>李清星</t>
   </si>
   <si>
+    <t>55%</t>
+  </si>
+  <si>
     <t>19020222202296</t>
   </si>
   <si>
     <t>李欣然</t>
   </si>
   <si>
+    <t>11%</t>
+  </si>
+  <si>
+    <t>85%</t>
+  </si>
+  <si>
+    <t>69%</t>
+  </si>
+  <si>
     <t>20420202201837</t>
   </si>
   <si>
     <t>徐清源</t>
   </si>
   <si>
+    <t>68%</t>
+  </si>
+  <si>
+    <t>81%</t>
+  </si>
+  <si>
     <t>25120212202184</t>
   </si>
   <si>
@@ -212,6 +362,9 @@
     <t>庄博诚</t>
   </si>
   <si>
+    <t>98%</t>
+  </si>
+  <si>
     <t>25120222201341</t>
   </si>
   <si>
@@ -239,6 +392,9 @@
     <t>程禹</t>
   </si>
   <si>
+    <t>93%</t>
+  </si>
+  <si>
     <t>37520222204672</t>
   </si>
   <si>
@@ -257,6 +413,9 @@
     <t>陈鸿达</t>
   </si>
   <si>
+    <t>82%</t>
+  </si>
+  <si>
     <t>37720222204905</t>
   </si>
   <si>
@@ -275,12 +434,18 @@
     <t>高源</t>
   </si>
   <si>
+    <t>74%</t>
+  </si>
+  <si>
     <t>37720222204939</t>
   </si>
   <si>
     <t>连传瀚</t>
   </si>
   <si>
+    <t>94%</t>
+  </si>
+  <si>
     <t>37720222204941</t>
   </si>
   <si>
@@ -335,24 +500,36 @@
     <t>张庄辉</t>
   </si>
   <si>
+    <t>84%</t>
+  </si>
+  <si>
     <t>37720222204990</t>
   </si>
   <si>
     <t>赵勤励</t>
   </si>
   <si>
+    <t>88%</t>
+  </si>
+  <si>
     <t>37720222204994</t>
   </si>
   <si>
     <t>周家辉</t>
   </si>
   <si>
+    <t>71%</t>
+  </si>
+  <si>
     <t>37720222204998</t>
   </si>
   <si>
     <t>卜於锴</t>
   </si>
   <si>
+    <t>91%</t>
+  </si>
+  <si>
     <t>37720222204999</t>
   </si>
   <si>
@@ -389,6 +566,9 @@
     <t>洪怡洁</t>
   </si>
   <si>
+    <t>96%</t>
+  </si>
+  <si>
     <t>37720222205026</t>
   </si>
   <si>
@@ -411,6 +591,9 @@
   </si>
   <si>
     <t>宋锐扬</t>
+  </si>
+  <si>
+    <t>79%</t>
   </si>
   <si>
     <t>37720222205078</t>
@@ -701,19 +884,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.79998168889431"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -725,19 +908,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.79998168889431"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -749,19 +932,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.79998168889431"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -773,19 +956,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.79998168889431"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -797,19 +980,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.79998168889431"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -821,19 +1004,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.79998168889431"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.5999938962981"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.39997558519242"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -875,7 +1058,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4" tint="0.49998474074526"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1627,22 +1810,25 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F1" sqref="F$1:F$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.75" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.9375" customWidth="1"/>
+    <col min="7" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1658,1200 +1844,2052 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H12" t="s">
         <v>25</v>
       </c>
-      <c r="C11" t="s">
+      <c r="I12" t="s">
         <v>26</v>
       </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>65</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>32</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>75</v>
+      </c>
+      <c r="G17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>78</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="H18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
       <c r="C19" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" t="s">
+        <v>82</v>
+      </c>
+      <c r="I19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>85</v>
       </c>
       <c r="D20" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" t="s">
+        <v>32</v>
+      </c>
+      <c r="H20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I20" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>87</v>
       </c>
       <c r="C21" t="s">
-        <v>46</v>
+        <v>88</v>
       </c>
       <c r="D21" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" t="s">
+        <v>32</v>
+      </c>
+      <c r="I21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>94</v>
+      </c>
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>96</v>
       </c>
       <c r="D24" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" t="s">
+        <v>24</v>
+      </c>
+      <c r="I24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>99</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>100</v>
+      </c>
+      <c r="G25" t="s">
+        <v>50</v>
+      </c>
+      <c r="H25" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>20</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>59</v>
+        <v>109</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>110</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>111</v>
+      </c>
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>61</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>62</v>
+        <v>113</v>
       </c>
       <c r="D29" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+        <v>114</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29" t="s">
+        <v>14</v>
+      </c>
+      <c r="H29" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
       <c r="C30" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F30" t="s">
+        <v>101</v>
+      </c>
+      <c r="G30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
-        <v>67</v>
+        <v>118</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>50</v>
+      </c>
+      <c r="G31" t="s">
+        <v>19</v>
+      </c>
+      <c r="H31" t="s">
+        <v>32</v>
+      </c>
+      <c r="I31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>120</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>121</v>
+      </c>
+      <c r="G32" t="s">
+        <v>59</v>
+      </c>
+      <c r="H32" t="s">
+        <v>42</v>
+      </c>
+      <c r="I32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>122</v>
       </c>
       <c r="C33" t="s">
-        <v>71</v>
+        <v>123</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F33" t="s">
+        <v>94</v>
+      </c>
+      <c r="G33" t="s">
+        <v>24</v>
+      </c>
+      <c r="H33" t="s">
+        <v>42</v>
+      </c>
+      <c r="I33" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>72</v>
+        <v>124</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" t="s">
+        <v>24</v>
+      </c>
+      <c r="I34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>74</v>
+        <v>126</v>
       </c>
       <c r="C35" t="s">
-        <v>75</v>
+        <v>127</v>
       </c>
       <c r="D35" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>128</v>
+      </c>
+      <c r="G35" t="s">
+        <v>24</v>
+      </c>
+      <c r="H35" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>129</v>
       </c>
       <c r="C36" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="D36" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E36" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>114</v>
+      </c>
+      <c r="F36" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" t="s">
+        <v>37</v>
+      </c>
+      <c r="I36" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>78</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="D37" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F37" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" t="s">
+        <v>32</v>
+      </c>
+      <c r="H37" t="s">
+        <v>101</v>
+      </c>
+      <c r="I37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>80</v>
+        <v>133</v>
       </c>
       <c r="C38" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>135</v>
+      </c>
+      <c r="G38" t="s">
+        <v>19</v>
+      </c>
+      <c r="H38" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>82</v>
+        <v>136</v>
       </c>
       <c r="C39" t="s">
-        <v>83</v>
+        <v>137</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>17</v>
+      </c>
+      <c r="G39" t="s">
+        <v>24</v>
+      </c>
+      <c r="H39" t="s">
+        <v>24</v>
+      </c>
+      <c r="I39" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>84</v>
+        <v>139</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>140</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F40" t="s">
+        <v>94</v>
+      </c>
+      <c r="G40" t="s">
+        <v>32</v>
+      </c>
+      <c r="H40" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
       <c r="C41" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="D41" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F41" t="s">
+        <v>24</v>
+      </c>
+      <c r="G41" t="s">
+        <v>32</v>
+      </c>
+      <c r="H41" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="C42" t="s">
-        <v>89</v>
+        <v>144</v>
       </c>
       <c r="D42" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F42" t="s">
+        <v>94</v>
+      </c>
+      <c r="G42" t="s">
+        <v>24</v>
+      </c>
+      <c r="H42" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>145</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>146</v>
       </c>
       <c r="D43" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F43" t="s">
+        <v>43</v>
+      </c>
+      <c r="G43" t="s">
+        <v>72</v>
+      </c>
+      <c r="H43" t="s">
+        <v>72</v>
+      </c>
+      <c r="I43" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>147</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>148</v>
       </c>
       <c r="D44" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>128</v>
+      </c>
+      <c r="G44" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" t="s">
+        <v>24</v>
+      </c>
+      <c r="I44" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="C45" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="D45" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" t="s">
+        <v>32</v>
+      </c>
+      <c r="H45" t="s">
+        <v>24</v>
+      </c>
+      <c r="I45" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>96</v>
+        <v>151</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>152</v>
       </c>
       <c r="D46" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F46" t="s">
+        <v>106</v>
+      </c>
+      <c r="G46" t="s">
+        <v>19</v>
+      </c>
+      <c r="H46" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>98</v>
+        <v>153</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>154</v>
       </c>
       <c r="D47" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F47" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" t="s">
+        <v>32</v>
+      </c>
+      <c r="H47" t="s">
+        <v>18</v>
+      </c>
+      <c r="I47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>100</v>
+        <v>155</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>156</v>
       </c>
       <c r="D48" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F48" t="s">
+        <v>157</v>
+      </c>
+      <c r="G48" t="s">
+        <v>32</v>
+      </c>
+      <c r="H48" t="s">
+        <v>72</v>
+      </c>
+      <c r="I48" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>158</v>
       </c>
       <c r="C49" t="s">
-        <v>103</v>
+        <v>159</v>
       </c>
       <c r="D49" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E49" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>114</v>
+      </c>
+      <c r="F49" t="s">
+        <v>160</v>
+      </c>
+      <c r="G49" t="s">
+        <v>37</v>
+      </c>
+      <c r="H49" t="s">
+        <v>19</v>
+      </c>
+      <c r="I49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>162</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>163</v>
+      </c>
+      <c r="G50" t="s">
+        <v>19</v>
+      </c>
+      <c r="H50" t="s">
+        <v>24</v>
+      </c>
+      <c r="I50" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>164</v>
       </c>
       <c r="C51" t="s">
-        <v>107</v>
+        <v>165</v>
       </c>
       <c r="D51" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>166</v>
+      </c>
+      <c r="G51" t="s">
+        <v>59</v>
+      </c>
+      <c r="H51" t="s">
+        <v>72</v>
+      </c>
+      <c r="I51" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52">
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>108</v>
+        <v>167</v>
       </c>
       <c r="C52" t="s">
-        <v>109</v>
+        <v>168</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F52" t="s">
+        <v>94</v>
+      </c>
+      <c r="G52" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" t="s">
+        <v>101</v>
+      </c>
+      <c r="I52" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>110</v>
+        <v>169</v>
       </c>
       <c r="C53" t="s">
-        <v>111</v>
+        <v>170</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>91</v>
+      </c>
+      <c r="G53" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" t="s">
+        <v>25</v>
+      </c>
+      <c r="I53" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>112</v>
+        <v>171</v>
       </c>
       <c r="C54" t="s">
-        <v>113</v>
+        <v>172</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E54" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+        <v>114</v>
+      </c>
+      <c r="F54" t="s">
+        <v>97</v>
+      </c>
+      <c r="G54" t="s">
+        <v>59</v>
+      </c>
+      <c r="H54" t="s">
+        <v>50</v>
+      </c>
+      <c r="I54" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
+        <v>173</v>
       </c>
       <c r="C55" t="s">
-        <v>115</v>
+        <v>174</v>
       </c>
       <c r="D55" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F55" t="s">
+        <v>26</v>
+      </c>
+      <c r="G55" t="s">
+        <v>24</v>
+      </c>
+      <c r="H55" t="s">
+        <v>24</v>
+      </c>
+      <c r="I55" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
       <c r="A56">
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
       <c r="C56" t="s">
-        <v>117</v>
+        <v>176</v>
       </c>
       <c r="D56" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F56" t="s">
+        <v>102</v>
+      </c>
+      <c r="G56" t="s">
+        <v>101</v>
+      </c>
+      <c r="H56" t="s">
+        <v>24</v>
+      </c>
+      <c r="I56" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>118</v>
+        <v>177</v>
       </c>
       <c r="C57" t="s">
-        <v>119</v>
+        <v>178</v>
       </c>
       <c r="D57" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E57" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
+        <v>179</v>
+      </c>
+      <c r="G57" t="s">
+        <v>18</v>
+      </c>
+      <c r="H57" t="s">
+        <v>72</v>
+      </c>
+      <c r="I57" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="C58" t="s">
-        <v>121</v>
+        <v>181</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E58" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F58" t="s">
+        <v>58</v>
+      </c>
+      <c r="G58" t="s">
+        <v>32</v>
+      </c>
+      <c r="H58" t="s">
+        <v>42</v>
+      </c>
+      <c r="I58" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
       <c r="A59">
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>182</v>
       </c>
       <c r="C59" t="s">
-        <v>123</v>
+        <v>183</v>
       </c>
       <c r="D59" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E59" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
+        <v>160</v>
+      </c>
+      <c r="G59" t="s">
+        <v>24</v>
+      </c>
+      <c r="H59" t="s">
+        <v>101</v>
+      </c>
+      <c r="I59" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
       <c r="A60">
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
       <c r="C60" t="s">
-        <v>125</v>
+        <v>185</v>
       </c>
       <c r="D60" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E60" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F60" t="s">
+        <v>160</v>
+      </c>
+      <c r="G60" t="s">
+        <v>42</v>
+      </c>
+      <c r="H60" t="s">
+        <v>72</v>
+      </c>
+      <c r="I60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
       <c r="A61">
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="C61" t="s">
-        <v>127</v>
+        <v>187</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F61" t="s">
+        <v>188</v>
+      </c>
+      <c r="G61" t="s">
+        <v>59</v>
+      </c>
+      <c r="H61" t="s">
+        <v>32</v>
+      </c>
+      <c r="I61" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
       <c r="A62">
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>128</v>
+        <v>189</v>
       </c>
       <c r="C62" t="s">
-        <v>129</v>
+        <v>190</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E62" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F62" t="s">
+        <v>26</v>
+      </c>
+      <c r="G62" t="s">
+        <v>32</v>
+      </c>
+      <c r="H62" t="s">
+        <v>42</v>
+      </c>
+      <c r="I62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
+        <v>191</v>
       </c>
       <c r="C63" t="s">
-        <v>131</v>
+        <v>192</v>
       </c>
       <c r="D63" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E63" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F63" t="s">
+        <v>102</v>
+      </c>
+      <c r="G63" t="s">
+        <v>32</v>
+      </c>
+      <c r="H63" t="s">
+        <v>72</v>
+      </c>
+      <c r="I63" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>132</v>
+        <v>193</v>
       </c>
       <c r="C64" t="s">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E64" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F64" t="s">
+        <v>121</v>
+      </c>
+      <c r="G64" t="s">
+        <v>59</v>
+      </c>
+      <c r="H64" t="s">
+        <v>72</v>
+      </c>
+      <c r="I64" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>134</v>
+        <v>195</v>
       </c>
       <c r="C65" t="s">
-        <v>135</v>
+        <v>196</v>
       </c>
       <c r="D65" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E65" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>114</v>
+      </c>
+      <c r="F65" t="s">
+        <v>121</v>
+      </c>
+      <c r="G65" t="s">
+        <v>76</v>
+      </c>
+      <c r="H65" t="s">
+        <v>72</v>
+      </c>
+      <c r="I65" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>197</v>
       </c>
       <c r="C66" t="s">
-        <v>137</v>
+        <v>198</v>
       </c>
       <c r="D66" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E66" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F66" t="s">
+        <v>26</v>
+      </c>
+      <c r="G66" t="s">
+        <v>32</v>
+      </c>
+      <c r="H66" t="s">
+        <v>101</v>
+      </c>
+      <c r="I66" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>199</v>
       </c>
       <c r="C67" t="s">
-        <v>139</v>
+        <v>200</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E67" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F67" t="s">
+        <v>166</v>
+      </c>
+      <c r="G67" t="s">
+        <v>42</v>
+      </c>
+      <c r="H67" t="s">
+        <v>42</v>
+      </c>
+      <c r="I67" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>140</v>
+        <v>201</v>
       </c>
       <c r="C68" t="s">
-        <v>141</v>
+        <v>202</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F68" t="s">
+        <v>50</v>
+      </c>
+      <c r="G68" t="s">
+        <v>32</v>
+      </c>
+      <c r="H68" t="s">
+        <v>18</v>
+      </c>
+      <c r="I68" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69">
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>142</v>
+        <v>203</v>
       </c>
       <c r="C69" t="s">
-        <v>143</v>
+        <v>204</v>
       </c>
       <c r="D69" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E69" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F69" t="s">
+        <v>68</v>
+      </c>
+      <c r="G69" t="s">
+        <v>19</v>
+      </c>
+      <c r="H69" t="s">
+        <v>24</v>
+      </c>
+      <c r="I69" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70">
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>205</v>
       </c>
       <c r="C70" t="s">
-        <v>145</v>
+        <v>206</v>
       </c>
       <c r="D70" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E70" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+        <v>12</v>
+      </c>
+      <c r="F70" t="s">
+        <v>26</v>
+      </c>
+      <c r="G70" t="s">
+        <v>59</v>
+      </c>
+      <c r="H70" t="s">
+        <v>42</v>
+      </c>
+      <c r="I70" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71">
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>207</v>
       </c>
       <c r="C71" t="s">
-        <v>147</v>
+        <v>208</v>
       </c>
       <c r="D71" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E71" t="s">
-        <v>8</v>
+        <v>12</v>
+      </c>
+      <c r="F71" t="s">
+        <v>76</v>
+      </c>
+      <c r="G71" t="s">
+        <v>72</v>
+      </c>
+      <c r="H71" t="s">
+        <v>72</v>
+      </c>
+      <c r="I71" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="2:2">
       <c r="B73" t="s">
-        <v>148</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>